<commit_message>
updates for test 2 and 2a
</commit_message>
<xml_diff>
--- a/2018-11-15 qbic test 2.xlsx
+++ b/2018-11-15 qbic test 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/confocal/Desktop/2018-11-05 Demis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theresa/Documents/home-github/cellprofiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CB8973-4BFD-9A4E-9C1D-0BD4EC2067E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FA49F7-B0C1-AA4F-9A52-AAFA8DD9C2B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17180" yWindow="11140" windowWidth="27720" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="8220" windowWidth="24780" windowHeight="10480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2018-11-15 qbic test 2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>Image</t>
   </si>
@@ -38,6 +38,15 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>look to be actually 7 cells in the frame -- AP detected 2 false pos. too</t>
+  </si>
+  <si>
+    <t>Analyze particles based on bad mask</t>
   </si>
 </sst>
 </file>
@@ -881,7 +890,8 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -951,6 +961,12 @@
       <c r="B4">
         <v>15</v>
       </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
       <c r="E4">
         <v>16</v>
       </c>
@@ -962,6 +978,12 @@
       <c r="B5">
         <v>8</v>
       </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
       <c r="E5">
         <v>9</v>
       </c>
@@ -973,6 +995,12 @@
       <c r="B6">
         <v>12</v>
       </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="E6">
         <v>13</v>
       </c>
@@ -984,6 +1012,12 @@
       <c r="B7">
         <v>3</v>
       </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
       <c r="E7">
         <v>3</v>
       </c>
@@ -995,8 +1029,17 @@
       <c r="B8">
         <v>9</v>
       </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
       <c r="E8">
         <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1006,8 +1049,17 @@
       <c r="B9">
         <v>0</v>
       </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
       <c r="E9">
         <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1017,6 +1069,12 @@
       <c r="B10">
         <v>11</v>
       </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
       <c r="E10">
         <v>11</v>
       </c>
@@ -1027,6 +1085,12 @@
       </c>
       <c r="B11">
         <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
       </c>
       <c r="E11">
         <v>8</v>

</xml_diff>